<commit_message>
Code without slack variables with terminal costs
</commit_message>
<xml_diff>
--- a/trajectory_gen_mpc/TimeLine/Timeline.xlsx
+++ b/trajectory_gen_mpc/TimeLine/Timeline.xlsx
@@ -562,16 +562,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>666000</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>136800</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>225720</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>345600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>673920</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>108000</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>232920</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>300960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -580,8 +580,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="12250080" y="814680"/>
-          <a:ext cx="7920" cy="5767560"/>
+          <a:off x="14847840" y="642600"/>
+          <a:ext cx="7200" cy="5766840"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -633,7 +633,7 @@
   <dimension ref="A1:AMJ23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>